<commit_message>
mejora en el formato de descarga de pdf, csv y xlsx
</commit_message>
<xml_diff>
--- a/demo/ruta/al/directorio/diagnostico.xlsx
+++ b/demo/ruta/al/directorio/diagnostico.xlsx
@@ -17,7 +17,24 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>El texto describe dos pacientes, "Pepito" (que llamaremos Sebastián) y "Juan" (que llamaremos Lucho). Sebastián presenta múltiples factores de riesgo para enfermedad cardiovascular, mientras que Lucho presenta un perfil de salud cardiovascular mucho más favorable.&lt;br&gt;&lt;br&gt;&lt;b&gt;Análisis de Sebastián (Pepito):&lt;/b&gt;&lt;br&gt;&lt;br&gt;Sebastián, de 55 años, exhibe un cuadro preocupante.  Su colesterol total está elevado (250 mg/dL), con un LDL alto (160 mg/dL) y un HDL bajo (40 mg/dL).  Los triglicéridos también están elevados (200 mg/dL).  Su presión arterial de 150/95 mmHg indica hipertensión.  Un IMC de 30 lo clasifica como obeso.  El tabaquismo, el historial familiar de infarto, el sedentarismo y una dieta rica en grasas y azúcares agravan aún más su riesgo. Su nivel de glucosa en sangre de 130 mg/dL sugiere prediabetes o diabetes.  Finalmente, los síntomas como dolor en el pecho, fatiga, dificultad para respirar, mareos y palpitaciones cardíacas pueden indicar problemas cardíacos subyacentes y requieren evaluación inmediata.&lt;br&gt;&lt;br&gt;&lt;b&gt;Diagnóstico presuntivo para Sebastián:&lt;/b&gt;  Alto riesgo de enfermedad cardiovascular. Posible angina de pecho, posiblemente relacionada con enfermedad arterial coronaria.  Necesita evaluación urgente para descartar isquemia miocárdica (falta de flujo sanguíneo al corazón).  También debe ser evaluado para diabetes.&lt;br&gt;&lt;br&gt;&lt;b&gt;Análisis de Lucho (Juan):&lt;/b&gt;&lt;br&gt;&lt;br&gt;Lucho, de 35 años, presenta un perfil lipídico saludable, presión arterial normal, un IMC normal y no fuma.  La ausencia de antecedentes familiares de enfermedad cardíaca es un factor positivo.  En general, tiene un bajo riesgo de enfermedad cardiovascular.&lt;br&gt;&lt;br&gt;&lt;b&gt;Diagnóstico para Lucho:&lt;/b&gt;  Bajo riesgo cardiovascular.  Se recomienda mantener hábitos de vida saludables.&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Recomendaciones para Sebastián:&lt;/b&gt;&lt;br&gt;&lt;br&gt;* &lt;b&gt;Evaluación médica urgente:&lt;/b&gt;  Debe consultar a un cardiólogo de inmediato para evaluar sus síntomas y realizar pruebas diagnósticas como electrocardiograma, prueba de esfuerzo y posiblemente un cateterismo cardíaco.&lt;br&gt;* &lt;b&gt;Modificación del estilo de vida:&lt;/b&gt;&lt;br&gt;    * Dejar de fumar inmediatamente.&lt;br&gt;    * Adoptar una dieta baja en grasas saturadas, colesterol y azúcares, rica en frutas, verduras y granos integrales.&lt;br&gt;    * Iniciar un programa de ejercicio regular, aprobado por su médico.&lt;br&gt;    * Controlar su peso.&lt;br&gt;* &lt;b&gt;Tratamiento farmacológico:&lt;/b&gt;  Probablemente necesite medicamentos para controlar la presión arterial, el colesterol y posiblemente la glucosa en sangre.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si Sebastián sigue las recomendaciones:&lt;/b&gt;  Puede reducir significativamente su riesgo de eventos cardiovasculares como infarto de miocardio o accidente cerebrovascular.  Mejorará su calidad de vida y su pronóstico a largo plazo.&lt;br&gt;&lt;br&gt;&lt;b&gt;Si Sebastián no sigue las recomendaciones:&lt;/b&gt;  Tiene un riesgo muy alto de sufrir un evento cardiovascular mayor, posiblemente con consecuencias graves o incluso fatales.  Su calidad de vida se verá afectada y su esperanza de vida podría reducirse.&lt;br&gt;&lt;br&gt;&lt;b&gt;Recomendaciones para Lucho:&lt;/b&gt;&lt;br&gt;&lt;br&gt;* Mantener una dieta saludable.&lt;br&gt;* Hacer ejercicio regularmente.&lt;br&gt;* No fumar.&lt;br&gt;* Controlar su presión arterial y colesterol periódicamente.&lt;br&gt;&lt;br&gt;&lt;br&gt;Las descripciones de las imágenes, "Pharmaceutical drug, Prescription drug, Pill, Screenshot," sugieren que se muestran medicamentos.  Sin embargo, sin ver las imágenes, no puedo comentar específicamente sobre ellas.  Es importante recordar que &lt;b&gt;nunca se debe automedicar&lt;/b&gt;.  Todo medicamento debe ser prescrito y supervisado por un médico.&lt;br&gt;</t>
+    <t xml:space="preserve">El paciente Pepito, de 55 años, presenta un riesgo cardiovascular significativamente alto.  Analicemos sus factores de riesgo:
+* Hipercolesterolemia: Su colesterol total (250 mg/dL), LDL (160 mg/dL) y triglicéridos (200 mg/dL) están elevados, mientras que su HDL (40 mg/dL) es bajo.  Esto favorece la formación de placas de ateroma en las arterias.
+* Hipertensión arterial: 150/95 mmHg es hipertensión estadio 2.  Aumenta la carga de trabajo del corazón y daña las arterias.
+* Obesidad: Un IMC de 30 lo clasifica como obeso, lo que contribuye a la hipertensión, la dislipidemia y la resistencia a la insulina.
+* Tabaquismo: Factor de riesgo mayor para enfermedad coronaria,  acelera el desarrollo de la aterosclerosis.
+* Historial familiar:  El infarto de su padre a los 60 años sugiere una predisposición genética.
+* Sedentarismo: La falta de actividad física agrava otros factores de riesgo.
+* Dieta inadecuada: Rica en grasas y azúcares contribuye a la obesidad, la dislipidemia y la diabetes.
+* Hiperglucemia:  Una glucosa de 130 mg/dL sugiere prediabetes o diabetes, otro factor de riesgo cardiovascular importante.
+* Síntomas: El dolor en el pecho, la fatiga, la disnea, los mareos y las palpitaciones son altamente sugestivos de angina de pecho,  posiblemente debido a isquemia miocárdica.
+Diagnóstico Presuntivo:  Angina estable con alto riesgo cardiovascular. Se requiere evaluación cardiológica urgente, incluyendo electrocardiograma, prueba de esfuerzo y posiblemente una angiografía coronaria, para descartar enfermedad arterial coronaria significativa.
+Recomendaciones:
+* Modificación agresiva del estilo de vida:  Dieta baja en grasas saturadas, colesterol, sodio y azúcares, rica en frutas, verduras y fibra.  Ejercicio aeróbico regular (al menos 30 minutos la mayoría de los días de la semana).  Cese inmediato del tabaquismo.
+* Tratamiento farmacológico:  Estatinas para reducir el colesterol LDL, antihipertensivos para controlar la presión arterial,  posiblemente antiplaquetarios (como aspirina) para prevenir la formación de coágulos, y  medicamentos para controlar la glucosa si se confirma la diabetes.
+Si sigue las recomendaciones:  Pepito puede reducir significativamente su riesgo cardiovascular, mejorar sus síntomas y su calidad de vida, y potencialmente prevenir eventos cardiovasculares mayores como un infarto de miocardio o un accidente cerebrovascular.
+Si no sigue las recomendaciones:  Pepito tiene un alto riesgo de sufrir complicaciones cardiovasculares graves, incluyendo infarto de miocardio, angina inestable, accidente cerebrovascular, insuficiencia cardíaca, e incluso muerte prematura.
+En cuanto a Juan, su perfil de riesgo es bajo, con valores normales de lípidos, presión arterial y IMC, ausencia de tabaquismo y sin antecedentes familiares.  La descripción de las imágenes como "píldoras" no aporta información relevante para el análisis.  La comparación sirve para ilustrar la diferencia entre un perfil de riesgo saludable y uno de alto riesgo.
+</t>
   </si>
 </sst>
 </file>
@@ -54,8 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -67,6 +87,9 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -74,7 +97,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
analisis de archivos pdf
</commit_message>
<xml_diff>
--- a/demo/ruta/al/directorio/diagnostico.xlsx
+++ b/demo/ruta/al/directorio/diagnostico.xlsx
@@ -17,23 +17,27 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t xml:space="preserve">El paciente Pepito, de 55 años, presenta un riesgo cardiovascular significativamente alto.  Analicemos sus factores de riesgo:
-* Hipercolesterolemia: Su colesterol total (250 mg/dL), LDL (160 mg/dL) y triglicéridos (200 mg/dL) están elevados, mientras que su HDL (40 mg/dL) es bajo.  Esto favorece la formación de placas de ateroma en las arterias.
-* Hipertensión arterial: 150/95 mmHg es hipertensión estadio 2.  Aumenta la carga de trabajo del corazón y daña las arterias.
-* Obesidad: Un IMC de 30 lo clasifica como obeso, lo que contribuye a la hipertensión, la dislipidemia y la resistencia a la insulina.
-* Tabaquismo: Factor de riesgo mayor para enfermedad coronaria,  acelera el desarrollo de la aterosclerosis.
-* Historial familiar:  El infarto de su padre a los 60 años sugiere una predisposición genética.
-* Sedentarismo: La falta de actividad física agrava otros factores de riesgo.
-* Dieta inadecuada: Rica en grasas y azúcares contribuye a la obesidad, la dislipidemia y la diabetes.
-* Hiperglucemia:  Una glucosa de 130 mg/dL sugiere prediabetes o diabetes, otro factor de riesgo cardiovascular importante.
-* Síntomas: El dolor en el pecho, la fatiga, la disnea, los mareos y las palpitaciones son altamente sugestivos de angina de pecho,  posiblemente debido a isquemia miocárdica.
-Diagnóstico Presuntivo:  Angina estable con alto riesgo cardiovascular. Se requiere evaluación cardiológica urgente, incluyendo electrocardiograma, prueba de esfuerzo y posiblemente una angiografía coronaria, para descartar enfermedad arterial coronaria significativa.
+    <t xml:space="preserve">Análisis del perfil de Juan:
+Los resultados de Juan indican un excelente estado de salud cardiovascular. Desglosemos cada valor:
+* Colesterol Total (180 mg/dL): Dentro del rango deseable (menor a 200 mg/dL).
+* Colesterol HDL (65 mg/dL):  Excelente nivel. El HDL, o colesterol "bueno", ayuda a eliminar el colesterol de las arterias, y un nivel superior a 60 mg/dL es protector.
+* Colesterol LDL (90 mg/dL): Óptimo.  El LDL, o colesterol "malo", contribuye a la acumulación de placa en las arterias. Mantenerlo bajo es crucial para la salud cardiovascular.
+* Triglicéridos (110 mg/dL):  Normal (deseable menos de 150 mg/dL).  Niveles elevados de triglicéridos pueden aumentar el riesgo de enfermedades del corazón.
+* Presión Arterial (120/80 mmHg):  Ideal.  Indica una presión arterial saludable y un bajo riesgo de hipertensión.
+* Índice de Masa Corporal (IMC) (23):  Dentro del rango de peso saludable.  Un IMC saludable reduce el riesgo de enfermedades cardíacas, diabetes y otras afecciones.
+* No fumador:  Factor crucial para la salud cardiovascular. El tabaco daña las arterias y aumenta significativamente el riesgo de enfermedades cardíacas.
+* Sin antecedentes familiares de enfermedades cardíacas: Aunque positivo, no elimina completamente el riesgo, ya que el estilo de vida también juega un papel importante.
+Diagnóstico:
+Juan presenta un perfil de riesgo cardiovascular muy bajo.  Sus valores están dentro de los rangos saludables, y sus hábitos de vida (al menos los mencionados) son beneficiosos para su salud cardiovascular.
 Recomendaciones:
-* Modificación agresiva del estilo de vida:  Dieta baja en grasas saturadas, colesterol, sodio y azúcares, rica en frutas, verduras y fibra.  Ejercicio aeróbico regular (al menos 30 minutos la mayoría de los días de la semana).  Cese inmediato del tabaquismo.
-* Tratamiento farmacológico:  Estatinas para reducir el colesterol LDL, antihipertensivos para controlar la presión arterial,  posiblemente antiplaquetarios (como aspirina) para prevenir la formación de coágulos, y  medicamentos para controlar la glucosa si se confirma la diabetes.
-Si sigue las recomendaciones:  Pepito puede reducir significativamente su riesgo cardiovascular, mejorar sus síntomas y su calidad de vida, y potencialmente prevenir eventos cardiovasculares mayores como un infarto de miocardio o un accidente cerebrovascular.
-Si no sigue las recomendaciones:  Pepito tiene un alto riesgo de sufrir complicaciones cardiovasculares graves, incluyendo infarto de miocardio, angina inestable, accidente cerebrovascular, insuficiencia cardíaca, e incluso muerte prematura.
-En cuanto a Juan, su perfil de riesgo es bajo, con valores normales de lípidos, presión arterial y IMC, ausencia de tabaquismo y sin antecedentes familiares.  La descripción de las imágenes como "píldoras" no aporta información relevante para el análisis.  La comparación sirve para ilustrar la diferencia entre un perfil de riesgo saludable y uno de alto riesgo.
+Aunque Juan está sano, es importante mantener estos hábitos saludables para prevenir futuras enfermedades.  Recomiendo:
+* Mantener una dieta equilibrada: Rica en frutas, verduras, granos integrales y baja en grasas saturadas y trans.
+* Ejercicio regular:  Al menos 150 minutos de actividad física moderada o 75 minutos de actividad vigorosa por semana.
+* Control regular de la salud:  Aunque esté sano, es importante realizarse chequeos médicos periódicos para controlar sus niveles de colesterol, presión arterial y otros indicadores de salud.
+¿Qué pasa si no sigue las recomendaciones?
+Si Juan abandona sus hábitos saludables (por ejemplo, comienza a fumar, adopta una dieta poco saludable o deja de hacer ejercicio), aumentará significativamente su riesgo de desarrollar enfermedades cardiovasculares en el futuro, como hipertensión,  enfermedad coronaria,  accidente cerebrovascular y otros problemas de salud.
+¿Qué pasa si sigue las recomendaciones?
+Si Juan mantiene su estilo de vida saludable,  tiene una alta probabilidad de mantener su bajo riesgo cardiovascular y disfrutar de una buena salud en el futuro.  Esto le permitirá reducir significativamente las posibilidades de desarrollar enfermedades cardíacas y mejorar su calidad de vida a largo plazo.
 </t>
   </si>
 </sst>

</xml_diff>